<commit_message>
Added test case of Empty City name or wrong properties Changed the test cases function name Updated unit test cases document
</commit_message>
<xml_diff>
--- a/documentations/3.1 Test Cases.xlsx
+++ b/documentations/3.1 Test Cases.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewzhu/Desktop/download/Massey/NZLife/CVs/cover letter/Westpac/assessment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewzhu/projects/SimpleWeatherInformationService/documentations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0321744F-C90B-F849-9D2E-CDEB8EA26F21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C75EDF8-694B-9949-B32A-8C4040573B95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="500" windowWidth="28040" windowHeight="16460" xr2:uid="{E915A98E-3771-FE4B-BA8D-90B67682E067}"/>
+    <workbookView xWindow="31640" yWindow="3540" windowWidth="28040" windowHeight="16420" xr2:uid="{E915A98E-3771-FE4B-BA8D-90B67682E067}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
     <sheet name="Test Evidence" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="67">
   <si>
     <t>No</t>
   </si>
@@ -72,9 +72,6 @@
     <t>SimpleWeatherInformationServiceApplicationTests</t>
   </si>
   <si>
-    <t>whenQueryWeatherRecordSuccessForOneCity</t>
-  </si>
-  <si>
     <t>[{"cityname":"Auckland"}]</t>
   </si>
   <si>
@@ -84,9 +81,6 @@
     <t>PASS</t>
   </si>
   <si>
-    <t>whenQueryWeatherRecordUnavailableForOneCity</t>
-  </si>
-  <si>
     <t>Test case for check the query result weather information, with date of 1 unavailable city</t>
   </si>
   <si>
@@ -96,43 +90,28 @@
     <t>Return with unfound tips</t>
   </si>
   <si>
-    <t>whenQueryWeatherRecordSuccessForThreeCities</t>
-  </si>
-  <si>
     <t>Test case for check the query result weather information, with data of 3 cities</t>
   </si>
   <si>
     <t>[{"cityname":"Auckland"},{"cityname":"Wellington"},{"cityname":"Hamilton"}]</t>
   </si>
   <si>
-    <t>whenQueryWeatherRecordSuccessForThreeCitiesWithOneUnavailable</t>
-  </si>
-  <si>
     <t>Test case for check the query result weather information, with data of 3 cities, 1 is unavailable</t>
   </si>
   <si>
     <t>Test case for check the query result weather information, with empty input</t>
   </si>
   <si>
-    <t>whenQueryWeatherRecordNoCityInput</t>
-  </si>
-  <si>
     <t>[]</t>
   </si>
   <si>
     <t>Test case for check the query result weather information, with data of 4 cities</t>
   </si>
   <si>
-    <t>whenQueryWeatherRecordMoreThanThreeCitiesInput</t>
-  </si>
-  <si>
     <t>[{"cityname":"Auckland"},{"cityname":"Wellington"},{"cityname":"Hamilton"},{"cityname":"Tauranga"}]</t>
   </si>
   <si>
     <t>Test case for check the query result weather information, with data of 1 city</t>
-  </si>
-  <si>
-    <t>whenQueryWeatherRecordSameCityInformationInput</t>
   </si>
   <si>
     <t>[{"cityname":"Auckland"},{"cityname":"Auckland"}]</t>
@@ -158,17 +137,11 @@
 	 when call queryWeatherByCities method</t>
   </si>
   <si>
-    <t>whenQueryWeatherRecordGetDaoException</t>
-  </si>
-  <si>
     <t>Test case between weatherInformationService and WeatherInformationController,
 	 make sure ServiceException can be thrown to WeatherInformationController from weatherInformationService
 	 when call queryWeatherByCities method</t>
   </si>
   <si>
-    <t>whenQueryWeatherRecordGetServiceException</t>
-  </si>
-  <si>
     <t>Return Massage with error information</t>
   </si>
   <si>
@@ -182,33 +155,21 @@
 	 when call getAvailableCities method</t>
   </si>
   <si>
-    <t>whenQueryAvaibleCitiesGetDaoException</t>
-  </si>
-  <si>
     <t>Test case between weatherInformationService and WeatherInformationController,
 	 make sure unknown exceptions can be thrown to weatherInformationService from weatherRecordDAO
 	 when call getAvailableCities method</t>
   </si>
   <si>
-    <t>whenQueryAvaibleCitiesGetUnknownException</t>
-  </si>
-  <si>
     <t>Test case between weatherInformationService and weatherRecordDAO,
 	 make sure  DataQueryException can be thrown to weatherInformationService from weatherRecordDAO
 	 when call getAvailableCities method</t>
   </si>
   <si>
-    <t>whenQueryAvaibleCitiesServiceGetDataQueryException</t>
-  </si>
-  <si>
     <t>Test case between weatherInformationService and weatherRecordDAO,
 	 make sure unknown exceptions can be thrown to weatherInformationService from weatherRecordDAO
 	 when call getAvailableCities method</t>
   </si>
   <si>
-    <t>whenQueryAvaibleCitiesServiceGetException</t>
-  </si>
-  <si>
     <t>Throw Exception in Service layer</t>
   </si>
   <si>
@@ -217,26 +178,86 @@
 	 when call queryWeatherByCities method</t>
   </si>
   <si>
-    <t>whenQueryWeatherRecordServiceGetDataQueryException</t>
-  </si>
-  <si>
     <t>Test case between weatherInformationService and weatherRecordDAO,
 	 make sure unknown exceptions can be thrown weatherInformationService from weatherRecordDAO
 	 when call queryWeatherByCities method</t>
   </si>
   <si>
-    <t>whenQueryWeatherRecordServiceGetUnknownException</t>
-  </si>
-  <si>
-    <t>whenQueryWeatherRecordGetUnknowException</t>
-  </si>
-  <si>
-    <t>whenQueryAvaibleCitiesGetServiceException</t>
-  </si>
-  <si>
     <t>Test case between weatherInformationService and WeatherInformationController,
 	 make sure unknown exceptions can be thrown to WeatherInformationController from weatherInformationService
 	 when call queryWeatherByCities method</t>
+  </si>
+  <si>
+    <t>Test case for input JSON contain empty city names</t>
+  </si>
+  <si>
+    <t>Test case with input with  wrong properties</t>
+  </si>
+  <si>
+    <t>[ {"cityname": "Auckland"},{"cityname": ""} ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[  {"cityname": "Auckland"},{"name": "Wellington"},{"city": "Hamilton"}  </t>
+  </si>
+  <si>
+    <t>Return with error of Wrong format</t>
+  </si>
+  <si>
+    <t>whenQueryWeatherInformationWithWrongPropertiesName</t>
+  </si>
+  <si>
+    <t>whenQueryWeatherInformationWithEmptyName</t>
+  </si>
+  <si>
+    <t>whenQueryWeatherInformationWithInputHasSameCityName</t>
+  </si>
+  <si>
+    <t>whenQueryWeatherInformationWithMoreThanThreeCitiesInput</t>
+  </si>
+  <si>
+    <t>whenQueryWeatherInformationWithThreeCitiesIncludedOneUnavailable</t>
+  </si>
+  <si>
+    <t>whenQueryQueryWeatherInformationWithThreeAvailableCities</t>
+  </si>
+  <si>
+    <t>whenQueryQueryWeatherInformationWithOneUnavailableCity</t>
+  </si>
+  <si>
+    <t>whenQueryWeatherInformationWithOneAvailableCity</t>
+  </si>
+  <si>
+    <t>whenQueryWeatherInformationWithNoInput</t>
+  </si>
+  <si>
+    <t>whenQueryWeatherInformationControllerGotDaoExceptionFromService</t>
+  </si>
+  <si>
+    <t>whenQueryWeatherInformationControllerGotServiceExceptionFromService</t>
+  </si>
+  <si>
+    <t>whenQueryWeatherInformationControllerGotUnknownExceptionFromService</t>
+  </si>
+  <si>
+    <t>whenQueryAvailableCitiesControllerGotServiceExceptionFromService</t>
+  </si>
+  <si>
+    <t>whenQueryAvailableCitiesControllerFotUnknownExceptionFromService</t>
+  </si>
+  <si>
+    <t>whenQueryAvailableCitiesServiceGotDataQueryExceptionFromDao</t>
+  </si>
+  <si>
+    <t>whenQueryAvailableCitiesServiceGotUnknownExceptionFromDao</t>
+  </si>
+  <si>
+    <t>whenQueryWeatherInformationServiceGotDataQueryExceptionFromDao</t>
+  </si>
+  <si>
+    <t>whenQueryWeatherInformationServiceGotUnknownExceptionFromDao</t>
+  </si>
+  <si>
+    <t>whenQueryAvailableCitiesControllerGotDataQueryExceptionFromService</t>
   </si>
 </sst>
 </file>
@@ -293,16 +314,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -319,9 +337,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -345,22 +360,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>180809</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>52308</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BBE53B1-18B8-136F-358F-D1CCB621DD67}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E75B38F-EA68-2544-8346-AE2FEB275C95}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -376,8 +391,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="7772400" cy="5464009"/>
+          <a:off x="812800" y="203200"/>
+          <a:ext cx="7772400" cy="6351508"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -706,16 +721,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD902BAD-E8E7-414D-B991-91F6E6284D27}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="60" style="2" customWidth="1"/>
-    <col min="3" max="3" width="51.83203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="66.83203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="69.33203125" style="2" customWidth="1"/>
     <col min="5" max="5" width="19.5" style="2" customWidth="1"/>
   </cols>
@@ -736,383 +751,420 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B3" s="4"/>
-    </row>
     <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>1</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>2</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="6">
+      <c r="C6" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>3</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>4</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
+        <v>5</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
+        <v>6</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
+        <v>7</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
+        <v>8</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
+        <v>9</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
+      <c r="B16" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="6">
+      <c r="D18" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="7" t="s">
+    </row>
+    <row r="19" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A19" s="4">
+        <v>1</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A20" s="4">
+        <v>2</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A21" s="4">
+        <v>3</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A22" s="4">
+        <v>4</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A23" s="4">
+        <v>5</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A24" s="4">
+        <v>6</v>
+      </c>
+      <c r="B24" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="6">
-        <v>5</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="6">
-        <v>6</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="6">
+      <c r="C24" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A25" s="4">
         <v>7</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="7" t="s">
+      <c r="B25" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="F25" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A26" s="4">
+        <v>8</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A27" s="4">
         <v>9</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="85" x14ac:dyDescent="0.2">
-      <c r="A17" s="5">
-        <v>1</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="7" t="s">
+      <c r="B27" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="85" x14ac:dyDescent="0.2">
-      <c r="A18" s="5">
-        <v>2</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" s="7" t="s">
+      <c r="F27" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A28" s="4">
+        <v>10</v>
+      </c>
+      <c r="B28" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="85" x14ac:dyDescent="0.2">
-      <c r="A19" s="5">
-        <v>3</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="85" x14ac:dyDescent="0.2">
-      <c r="A20" s="5">
-        <v>4</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="85" x14ac:dyDescent="0.2">
-      <c r="A21" s="5">
-        <v>5</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="85" x14ac:dyDescent="0.2">
-      <c r="A22" s="5">
-        <v>6</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="85" x14ac:dyDescent="0.2">
-      <c r="A23" s="5">
-        <v>7</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="85" x14ac:dyDescent="0.2">
-      <c r="A24" s="10">
-        <v>8</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="85" x14ac:dyDescent="0.2">
-      <c r="A25" s="10">
-        <v>9</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="85" x14ac:dyDescent="0.2">
-      <c r="A26" s="10">
-        <v>10</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>14</v>
+      <c r="C28" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1125,7 +1177,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update test cases for customized error handle of method not support and not found exception
</commit_message>
<xml_diff>
--- a/documentations/3.1 Test Cases.xlsx
+++ b/documentations/3.1 Test Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewzhu/projects/SimpleWeatherInformationService/documentations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C75EDF8-694B-9949-B32A-8C4040573B95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD8DE66-9BF1-B042-854E-AEE12DCD0E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31640" yWindow="3540" windowWidth="28040" windowHeight="16420" xr2:uid="{E915A98E-3771-FE4B-BA8D-90B67682E067}"/>
+    <workbookView xWindow="28800" yWindow="2180" windowWidth="38400" windowHeight="21100" xr2:uid="{E915A98E-3771-FE4B-BA8D-90B67682E067}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="80">
   <si>
     <t>No</t>
   </si>
@@ -75,9 +75,6 @@
     <t>[{"cityname":"Auckland"}]</t>
   </si>
   <si>
-    <t>Normal return</t>
-  </si>
-  <si>
     <t>PASS</t>
   </si>
   <si>
@@ -87,9 +84,6 @@
     <t>[{\"cityname\":\"ChristChurch\"}]"</t>
   </si>
   <si>
-    <t>Return with unfound tips</t>
-  </si>
-  <si>
     <t>Test case for check the query result weather information, with data of 3 cities</t>
   </si>
   <si>
@@ -115,15 +109,6 @@
   </si>
   <si>
     <t>[{"cityname":"Auckland"},{"cityname":"Auckland"}]</t>
-  </si>
-  <si>
-    <t>Return with error of duplication</t>
-  </si>
-  <si>
-    <t>Return with tips of exceed</t>
-  </si>
-  <si>
-    <t>Return with tips of no input data</t>
   </si>
   <si>
     <t>[{"cityname":"Auckland"},{"cityname":"Wellington"},{"cityname":"ChristChurch"}]</t>
@@ -142,9 +127,6 @@
 	 when call queryWeatherByCities method</t>
   </si>
   <si>
-    <t>Return Massage with error information</t>
-  </si>
-  <si>
     <t>Test case between weatherInformationService and WeatherInformationController,
 	 make sure ServiceException can be thrown to WeatherInformationController from weatherInformationService
 	 when call getAvailableCities method</t>
@@ -200,9 +182,6 @@
     <t xml:space="preserve">[  {"cityname": "Auckland"},{"name": "Wellington"},{"city": "Hamilton"}  </t>
   </si>
   <si>
-    <t>Return with error of Wrong format</t>
-  </si>
-  <si>
     <t>whenQueryWeatherInformationWithWrongPropertiesName</t>
   </si>
   <si>
@@ -258,6 +237,66 @@
   </si>
   <si>
     <t>whenQueryAvailableCitiesControllerGotDataQueryExceptionFromService</t>
+  </si>
+  <si>
+    <t>whenQueryWeatherInformationNotUseGetMethod</t>
+  </si>
+  <si>
+    <t>Test case for call /queryweatherbycities out of GET method, and POST method</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Test case for call /availablecities out of GET method, and POST method</t>
+  </si>
+  <si>
+    <t>whenQueryAvailableCitiesNotUseGetMethod</t>
+  </si>
+  <si>
+    <t>Normal return, whti HTTP status ok</t>
+  </si>
+  <si>
+    <t>Return with unfound tips, with HTTP status ok</t>
+  </si>
+  <si>
+    <t>Normal return, with HTTP status ok</t>
+  </si>
+  <si>
+    <t>Return with tips of no input data, with HTTP status bad request</t>
+  </si>
+  <si>
+    <t>Return with tips of exceed,with HTTP status bad request</t>
+  </si>
+  <si>
+    <t>Return with error of duplication,with HTTP status bad request</t>
+  </si>
+  <si>
+    <t>Return with error of wrong format, with HTTP status bad request</t>
+  </si>
+  <si>
+    <t>Return with error of Wrong format, with HTTP status bad request</t>
+  </si>
+  <si>
+    <t>Return Massage with error information, with HTTP status Internal Server Error</t>
+  </si>
+  <si>
+    <t>Return Massage with error information,  with HTTP status Internal Server Error</t>
+  </si>
+  <si>
+    <t>Return Massage with error information, , with HTTP status Internal Server Error</t>
+  </si>
+  <si>
+    <t>Test case for call not existed uri resource</t>
+  </si>
+  <si>
+    <t>whenQueryResourceNotFound</t>
+  </si>
+  <si>
+    <t>Return with error of Unsupport method, with HTTP status method not allowe</t>
+  </si>
+  <si>
+    <t>Return with error of Unsupport method, with HTTP status  method not allowe</t>
+  </si>
+  <si>
+    <t>Return with error of resource not found method, with HTTP status method NOT FOUND</t>
   </si>
 </sst>
 </file>
@@ -359,23 +398,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>812800</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>330200</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>52308</xdr:rowOff>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>144622</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E75B38F-EA68-2544-8346-AE2FEB275C95}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCB778B9-6B72-BF0F-8FB1-F08B393143E2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -391,8 +430,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="812800" y="203200"/>
-          <a:ext cx="7772400" cy="6351508"/>
+          <a:off x="825500" y="203200"/>
+          <a:ext cx="7772400" cy="7053422"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -721,10 +760,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD902BAD-E8E7-414D-B991-91F6E6284D27}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -732,7 +771,7 @@
     <col min="2" max="2" width="60" style="2" customWidth="1"/>
     <col min="3" max="3" width="66.83203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="69.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="19.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28.1640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -771,7 +810,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>1</v>
       </c>
@@ -779,16 +818,16 @@
         <v>7</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -796,19 +835,19 @@
         <v>2</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>15</v>
-      </c>
       <c r="E6" s="6" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -816,19 +855,19 @@
         <v>3</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -836,19 +875,19 @@
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -856,19 +895,19 @@
         <v>5</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -876,295 +915,353 @@
         <v>6</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>7</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>8</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <v>9</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
+        <v>10</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A15" s="5">
+        <v>11</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
+        <v>12</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B18" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+    <row r="19" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="7" t="s">
+      <c r="B19" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B21" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C21" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D21" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E21" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F21" s="7" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="85" x14ac:dyDescent="0.2">
-      <c r="A19" s="4">
-        <v>1</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="85" x14ac:dyDescent="0.2">
-      <c r="A20" s="4">
-        <v>2</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="85" x14ac:dyDescent="0.2">
-      <c r="A21" s="4">
-        <v>3</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="6" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="6" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="6" t="s">
-        <v>33</v>
+        <v>74</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="6" t="s">
-        <v>33</v>
+        <v>74</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="6" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="6" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="6" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A29" s="4">
+        <v>8</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A30" s="4">
+        <v>9</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A31" s="4">
+        <v>10</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1177,7 +1274,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>